<commit_message>
experiment with new stimuli
</commit_message>
<xml_diff>
--- a/stimuli/df_with_validity_checks_2024_Tomi_selected.xlsx
+++ b/stimuli/df_with_validity_checks_2024_Tomi_selected.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dameliotomas\experiment_VR\stimuli\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D45E3481-B178-42CF-80A2-3169ED9C3950}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3B2EC89-6879-43F0-8B0D-B3B11972C804}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7815" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="11625" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -842,9 +842,74 @@
     <t>Tiene buena variabilidad por ser arousal bajo. Eso me gusta.</t>
   </si>
   <si>
+    <t>Video de altura (Es simulacion, pero esta bueno). Lo termino sacando porque es el unico que es simulado, y prefiero el resto de los videos. Ademas ya tengo otro de altura.</t>
+  </si>
+  <si>
+    <t>00:00- 02:04</t>
+  </si>
+  <si>
+    <t>00:34- 03:08</t>
+  </si>
+  <si>
+    <t>The emotional content is the sport, not what they say. Sin embargo, hablan bastante. Decidir que hacer con eso</t>
+  </si>
+  <si>
+    <t>Hablan bastante. Decidir que hacer con eso</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Da mucho asco (eso es algo bueno). Pero la calidad es bastante mala de los videos. Capaz se puede seleccionar algunos. </t>
+  </si>
+  <si>
+    <t>Los pandas son muy tiernos. Hay que recortar alguna parte del video (nos permite flexibilidad para que todos los cuadrantes nos queden iguales). Arranca en el 00:06. En 01:59 podria haber un corte. 5 12  a 7:02</t>
+  </si>
+  <si>
+    <t>05:12- 07:02</t>
+  </si>
+  <si>
+    <t>00:00- 02:51</t>
+  </si>
+  <si>
+    <t>00:10- 02:40</t>
+  </si>
+  <si>
+    <t>00:05- 02:15</t>
+  </si>
+  <si>
+    <t>01:50- 02:50</t>
+  </si>
+  <si>
+    <t>00:00- 02:58</t>
+  </si>
+  <si>
+    <t>00:07- 03:11</t>
+  </si>
+  <si>
+    <t>00:00- 02:18</t>
+  </si>
+  <si>
+    <t>00:10- 02:26</t>
+  </si>
+  <si>
+    <t>00:00- 03:36</t>
+  </si>
+  <si>
+    <t>00:06- 03:00</t>
+  </si>
+  <si>
+    <t>00:04- 01:30</t>
+  </si>
+  <si>
+    <t>00:35- 02:17</t>
+  </si>
+  <si>
+    <t>Exp_video</t>
+  </si>
+  <si>
+    <t>Calm_video</t>
+  </si>
+  <si>
     <r>
       <rPr>
-        <b/>
         <sz val="11"/>
         <color theme="6" tint="-0.249977111117893"/>
         <rFont val="Calibri"/>
@@ -855,7 +920,6 @@
     </r>
     <r>
       <rPr>
-        <b/>
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
@@ -868,7 +932,6 @@
   <si>
     <r>
       <rPr>
-        <b/>
         <sz val="11"/>
         <color theme="6" tint="-0.249977111117893"/>
         <rFont val="Calibri"/>
@@ -878,7 +941,6 @@
     </r>
     <r>
       <rPr>
-        <b/>
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
@@ -887,82 +949,23 @@
       <t xml:space="preserve"> Buena varibailidad.</t>
     </r>
   </si>
-  <si>
-    <t>Video de altura (Es simulacion, pero esta bueno). Lo termino sacando porque es el unico que es simulado, y prefiero el resto de los videos. Ademas ya tengo otro de altura.</t>
-  </si>
-  <si>
-    <t>00:00- 02:04</t>
-  </si>
-  <si>
-    <t>00:34- 03:08</t>
-  </si>
-  <si>
-    <t>The emotional content is the sport, not what they say. Sin embargo, hablan bastante. Decidir que hacer con eso</t>
-  </si>
-  <si>
-    <t>Hablan bastante. Decidir que hacer con eso</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Da mucho asco (eso es algo bueno). Pero la calidad es bastante mala de los videos. Capaz se puede seleccionar algunos. </t>
-  </si>
-  <si>
-    <t>Los pandas son muy tiernos. Hay que recortar alguna parte del video (nos permite flexibilidad para que todos los cuadrantes nos queden iguales). Arranca en el 00:06. En 01:59 podria haber un corte. 5 12  a 7:02</t>
-  </si>
-  <si>
-    <t>05:12- 07:02</t>
-  </si>
-  <si>
-    <t>00:00- 02:51</t>
-  </si>
-  <si>
-    <t>00:10- 02:40</t>
-  </si>
-  <si>
-    <t>00:05- 02:15</t>
-  </si>
-  <si>
-    <t>01:50- 02:50</t>
-  </si>
-  <si>
-    <t>00:00- 02:58</t>
-  </si>
-  <si>
-    <t>00:07- 03:11</t>
-  </si>
-  <si>
-    <t>00:00- 02:18</t>
-  </si>
-  <si>
-    <t>00:10- 02:26</t>
-  </si>
-  <si>
-    <t>00:00- 03:36</t>
-  </si>
-  <si>
-    <t>00:06- 03:00</t>
-  </si>
-  <si>
-    <t>00:04- 01:30</t>
-  </si>
-  <si>
-    <t>00:35- 02:17</t>
-  </si>
-  <si>
-    <t>Exp_video</t>
-  </si>
-  <si>
-    <t>Calm_video</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="31" x14ac:knownFonts="1">
+  <fonts count="29" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1064,26 +1067,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color theme="10"/>
       <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
@@ -1122,44 +1109,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="6" tint="-0.249977111117893"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="6" tint="-0.249977111117893"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -1175,8 +1126,34 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="6" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="6" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1217,6 +1194,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
         <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor rgb="FFD99594"/>
       </patternFill>
     </fill>
   </fills>
@@ -1306,149 +1289,130 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="22" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="20" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="24" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="25" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="25" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="24" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="25" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="26" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="23" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="20" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="26" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="30" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="24" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1676,7 +1640,7 @@
     <col min="1" max="1" width="6.86328125" customWidth="1"/>
     <col min="2" max="2" width="8.06640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.06640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.3984375" customWidth="1"/>
     <col min="5" max="5" width="8.06640625" customWidth="1"/>
     <col min="6" max="6" width="73.1328125" customWidth="1"/>
     <col min="7" max="7" width="19.265625" customWidth="1"/>
@@ -1703,16 +1667,16 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="55" t="s">
+      <c r="B1" s="43" t="s">
         <v>242</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>290</v>
-      </c>
-      <c r="E1" s="55" t="s">
+        <v>288</v>
+      </c>
+      <c r="E1" s="43" t="s">
         <v>259</v>
       </c>
       <c r="F1" s="1" t="s">
@@ -1910,26 +1874,26 @@
       </c>
     </row>
     <row r="4" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A4" s="65">
+      <c r="A4" s="4">
         <v>14</v>
       </c>
-      <c r="B4" s="65" t="s">
-        <v>27</v>
-      </c>
-      <c r="C4" s="65" t="s">
-        <v>27</v>
-      </c>
-      <c r="D4" s="68"/>
-      <c r="E4" s="65" t="s">
+      <c r="B4" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="56"/>
+      <c r="E4" s="4" t="s">
         <v>260</v>
       </c>
-      <c r="F4" s="71" t="s">
+      <c r="F4" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="G4" s="65" t="s">
+      <c r="G4" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="H4" s="65" t="s">
+      <c r="H4" s="4" t="s">
         <v>40</v>
       </c>
       <c r="I4" s="6" t="s">
@@ -1948,7 +1912,7 @@
       <c r="N4" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="O4" s="56" t="s">
+      <c r="O4" s="44" t="s">
         <v>42</v>
       </c>
       <c r="P4" s="8" t="s">
@@ -1960,8 +1924,8 @@
       <c r="R4" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="S4" s="79" t="s">
-        <v>280</v>
+      <c r="S4" s="51" t="s">
+        <v>278</v>
       </c>
       <c r="U4" s="8" t="s">
         <v>27</v>
@@ -2240,26 +2204,26 @@
       </c>
     </row>
     <row r="9" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A9" s="20">
+      <c r="A9" s="9">
         <v>25</v>
       </c>
-      <c r="B9" s="53" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" s="28" t="s">
-        <v>27</v>
-      </c>
-      <c r="D9" s="60"/>
-      <c r="E9" s="58" t="s">
+      <c r="B9" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="57"/>
+      <c r="E9" s="9" t="s">
         <v>261</v>
       </c>
-      <c r="F9" s="73" t="s">
+      <c r="F9" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="G9" s="20" t="s">
+      <c r="G9" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="H9" s="20" t="s">
+      <c r="H9" s="9" t="s">
         <v>266</v>
       </c>
       <c r="I9" s="6"/>
@@ -2276,7 +2240,7 @@
       <c r="N9" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="O9" s="56" t="s">
+      <c r="O9" s="44" t="s">
         <v>70</v>
       </c>
       <c r="P9" s="8" t="s">
@@ -2285,8 +2249,8 @@
       <c r="Q9" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="S9" s="79" t="s">
-        <v>286</v>
+      <c r="S9" s="51" t="s">
+        <v>284</v>
       </c>
       <c r="U9" s="8" t="s">
         <v>27</v>
@@ -2305,22 +2269,22 @@
       </c>
     </row>
     <row r="10" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="21">
-        <v>27</v>
-      </c>
-      <c r="B10" s="21"/>
-      <c r="C10" s="21"/>
-      <c r="D10" s="21"/>
+      <c r="A10" s="20">
+        <v>27</v>
+      </c>
+      <c r="B10" s="20"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="20"/>
       <c r="E10" s="9" t="s">
         <v>261</v>
       </c>
-      <c r="F10" s="22" t="s">
+      <c r="F10" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="G10" s="21" t="s">
+      <c r="G10" s="20" t="s">
         <v>72</v>
       </c>
-      <c r="H10" s="21" t="s">
+      <c r="H10" s="20" t="s">
         <v>73</v>
       </c>
       <c r="I10" s="6"/>
@@ -2337,7 +2301,7 @@
       <c r="N10" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="O10" s="23" t="s">
+      <c r="O10" s="22" t="s">
         <v>75</v>
       </c>
       <c r="P10" s="8" t="s">
@@ -2366,27 +2330,27 @@
       </c>
     </row>
     <row r="11" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="24">
+      <c r="A11" s="58">
         <v>28</v>
       </c>
-      <c r="B11" s="53" t="s">
-        <v>27</v>
-      </c>
-      <c r="C11" s="53"/>
-      <c r="D11" s="60" t="s">
-        <v>27</v>
-      </c>
-      <c r="E11" s="58" t="s">
+      <c r="B11" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="11"/>
+      <c r="D11" s="57" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" s="9" t="s">
         <v>261</v>
       </c>
-      <c r="F11" s="24" t="s">
+      <c r="F11" s="58" t="s">
         <v>76</v>
       </c>
-      <c r="G11" s="24" t="s">
+      <c r="G11" s="58" t="s">
         <v>31</v>
       </c>
-      <c r="H11" s="24" t="s">
-        <v>267</v>
+      <c r="H11" s="58" t="s">
+        <v>289</v>
       </c>
       <c r="I11" s="6"/>
       <c r="J11" s="7"/>
@@ -2402,7 +2366,7 @@
       <c r="N11" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="O11" s="56" t="s">
+      <c r="O11" s="44" t="s">
         <v>78</v>
       </c>
       <c r="P11" s="8" t="s">
@@ -2411,8 +2375,8 @@
       <c r="Q11" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="S11" s="79" t="s">
-        <v>283</v>
+      <c r="S11" s="51" t="s">
+        <v>281</v>
       </c>
       <c r="U11" s="8" t="s">
         <v>27</v>
@@ -2443,7 +2407,7 @@
       <c r="F12" s="19" t="s">
         <v>79</v>
       </c>
-      <c r="G12" s="25" t="s">
+      <c r="G12" s="23" t="s">
         <v>52</v>
       </c>
       <c r="H12" s="19" t="s">
@@ -2460,7 +2424,7 @@
       <c r="M12" s="8">
         <v>120</v>
       </c>
-      <c r="N12" s="77" t="s">
+      <c r="N12" s="49" t="s">
         <v>81</v>
       </c>
       <c r="O12" s="8" t="s">
@@ -2617,19 +2581,19 @@
       </c>
     </row>
     <row r="15" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A15" s="25">
+      <c r="A15" s="23">
         <v>35</v>
       </c>
-      <c r="B15" s="25"/>
-      <c r="C15" s="25"/>
-      <c r="D15" s="25"/>
+      <c r="B15" s="23"/>
+      <c r="C15" s="23"/>
+      <c r="D15" s="23"/>
       <c r="E15" s="9" t="s">
         <v>261</v>
       </c>
       <c r="F15" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="G15" s="25" t="s">
+      <c r="G15" s="23" t="s">
         <v>72</v>
       </c>
       <c r="H15" s="19" t="s">
@@ -2809,20 +2773,20 @@
       </c>
     </row>
     <row r="18" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A18" s="26">
+      <c r="A18" s="24">
         <v>39</v>
       </c>
-      <c r="B18" s="26"/>
-      <c r="C18" s="26"/>
-      <c r="D18" s="26"/>
-      <c r="E18" s="26"/>
-      <c r="F18" s="27" t="s">
+      <c r="B18" s="24"/>
+      <c r="C18" s="24"/>
+      <c r="D18" s="24"/>
+      <c r="E18" s="24"/>
+      <c r="F18" s="25" t="s">
         <v>107</v>
       </c>
-      <c r="G18" s="26" t="s">
+      <c r="G18" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="H18" s="26" t="s">
+      <c r="H18" s="24" t="s">
         <v>108</v>
       </c>
       <c r="I18" s="6"/>
@@ -2935,20 +2899,20 @@
       </c>
     </row>
     <row r="20" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A20" s="27">
+      <c r="A20" s="25">
         <v>41</v>
       </c>
-      <c r="B20" s="27"/>
-      <c r="C20" s="27"/>
-      <c r="D20" s="27"/>
-      <c r="E20" s="27"/>
-      <c r="F20" s="27" t="s">
+      <c r="B20" s="25"/>
+      <c r="C20" s="25"/>
+      <c r="D20" s="25"/>
+      <c r="E20" s="25"/>
+      <c r="F20" s="25" t="s">
         <v>116</v>
       </c>
-      <c r="G20" s="26" t="s">
+      <c r="G20" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="H20" s="26" t="s">
+      <c r="H20" s="24" t="s">
         <v>117</v>
       </c>
       <c r="I20" s="6"/>
@@ -3189,26 +3153,26 @@
       </c>
     </row>
     <row r="24" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A24" s="28">
+      <c r="A24" s="11">
         <v>46</v>
       </c>
-      <c r="B24" s="53" t="s">
-        <v>27</v>
-      </c>
-      <c r="C24" s="28" t="s">
-        <v>27</v>
-      </c>
-      <c r="D24" s="60"/>
-      <c r="E24" s="58" t="s">
+      <c r="B24" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D24" s="57"/>
+      <c r="E24" s="9" t="s">
         <v>261</v>
       </c>
-      <c r="F24" s="28" t="s">
+      <c r="F24" s="11" t="s">
         <v>135</v>
       </c>
-      <c r="G24" s="28" t="s">
+      <c r="G24" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="H24" s="28" t="s">
+      <c r="H24" s="11" t="s">
         <v>136</v>
       </c>
       <c r="I24" s="6"/>
@@ -3225,7 +3189,7 @@
       <c r="N24" s="8" t="s">
         <v>137</v>
       </c>
-      <c r="O24" s="56" t="s">
+      <c r="O24" s="44" t="s">
         <v>138</v>
       </c>
       <c r="P24" s="8" t="s">
@@ -3234,8 +3198,8 @@
       <c r="Q24" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="S24" s="79" t="s">
-        <v>281</v>
+      <c r="S24" s="51" t="s">
+        <v>279</v>
       </c>
       <c r="U24" s="8" t="s">
         <v>27</v>
@@ -3315,12 +3279,12 @@
       </c>
     </row>
     <row r="26" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A26" s="29">
+      <c r="A26" s="26">
         <v>51</v>
       </c>
-      <c r="B26" s="29"/>
-      <c r="C26" s="29"/>
-      <c r="D26" s="29"/>
+      <c r="B26" s="26"/>
+      <c r="C26" s="26"/>
+      <c r="D26" s="26"/>
       <c r="E26" s="9" t="s">
         <v>261</v>
       </c>
@@ -3376,22 +3340,22 @@
       </c>
     </row>
     <row r="27" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A27" s="30">
+      <c r="A27" s="27">
         <v>52</v>
       </c>
-      <c r="B27" s="49"/>
-      <c r="C27" s="31"/>
-      <c r="D27" s="31"/>
-      <c r="E27" s="48" t="s">
+      <c r="B27" s="41"/>
+      <c r="C27" s="28"/>
+      <c r="D27" s="28"/>
+      <c r="E27" s="40" t="s">
         <v>262</v>
       </c>
-      <c r="F27" s="30" t="s">
+      <c r="F27" s="27" t="s">
         <v>149</v>
       </c>
-      <c r="G27" s="30" t="s">
+      <c r="G27" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="H27" s="30" t="s">
+      <c r="H27" s="27" t="s">
         <v>150</v>
       </c>
       <c r="I27" s="6"/>
@@ -3437,22 +3401,22 @@
       </c>
     </row>
     <row r="28" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A28" s="31">
+      <c r="A28" s="28">
         <v>53</v>
       </c>
-      <c r="B28" s="31"/>
-      <c r="C28" s="31"/>
-      <c r="D28" s="31"/>
-      <c r="E28" s="48" t="s">
+      <c r="B28" s="28"/>
+      <c r="C28" s="28"/>
+      <c r="D28" s="28"/>
+      <c r="E28" s="40" t="s">
         <v>262</v>
       </c>
-      <c r="F28" s="30" t="s">
+      <c r="F28" s="27" t="s">
         <v>154</v>
       </c>
-      <c r="G28" s="32" t="s">
+      <c r="G28" s="29" t="s">
         <v>72</v>
       </c>
-      <c r="H28" s="32" t="s">
+      <c r="H28" s="29" t="s">
         <v>155</v>
       </c>
       <c r="I28" s="6"/>
@@ -3498,26 +3462,26 @@
       </c>
     </row>
     <row r="29" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A29" s="28">
+      <c r="A29" s="11">
         <v>54</v>
       </c>
-      <c r="B29" s="28" t="s">
-        <v>27</v>
-      </c>
-      <c r="C29" s="28" t="s">
-        <v>27</v>
-      </c>
-      <c r="D29" s="60"/>
-      <c r="E29" s="58" t="s">
+      <c r="B29" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C29" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D29" s="57"/>
+      <c r="E29" s="9" t="s">
         <v>261</v>
       </c>
-      <c r="F29" s="28" t="s">
+      <c r="F29" s="11" t="s">
         <v>159</v>
       </c>
-      <c r="G29" s="28" t="s">
+      <c r="G29" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="H29" s="28" t="s">
+      <c r="H29" s="11" t="s">
         <v>160</v>
       </c>
       <c r="I29" s="6"/>
@@ -3534,7 +3498,7 @@
       <c r="N29" s="8" t="s">
         <v>161</v>
       </c>
-      <c r="O29" s="56" t="s">
+      <c r="O29" s="44" t="s">
         <v>162</v>
       </c>
       <c r="P29" s="8" t="s">
@@ -3543,7 +3507,7 @@
       <c r="Q29" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="S29" s="79" t="s">
+      <c r="S29" s="51" t="s">
         <v>163</v>
       </c>
       <c r="U29" s="8" t="s">
@@ -3691,22 +3655,22 @@
       </c>
     </row>
     <row r="32" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A32" s="31">
+      <c r="A32" s="28">
         <v>64</v>
       </c>
-      <c r="B32" s="31"/>
-      <c r="C32" s="31"/>
-      <c r="D32" s="31"/>
-      <c r="E32" s="48" t="s">
+      <c r="B32" s="28"/>
+      <c r="C32" s="28"/>
+      <c r="D32" s="28"/>
+      <c r="E32" s="40" t="s">
         <v>262</v>
       </c>
-      <c r="F32" s="30" t="s">
+      <c r="F32" s="27" t="s">
         <v>175</v>
       </c>
-      <c r="G32" s="31" t="s">
+      <c r="G32" s="28" t="s">
         <v>176</v>
       </c>
-      <c r="H32" s="31" t="s">
+      <c r="H32" s="28" t="s">
         <v>177</v>
       </c>
       <c r="I32" s="6"/>
@@ -3752,20 +3716,20 @@
       </c>
     </row>
     <row r="33" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A33" s="31">
+      <c r="A33" s="28">
         <v>66</v>
       </c>
-      <c r="B33" s="31"/>
-      <c r="C33" s="31"/>
-      <c r="D33" s="31"/>
-      <c r="E33" s="48" t="s">
+      <c r="B33" s="28"/>
+      <c r="C33" s="28"/>
+      <c r="D33" s="28"/>
+      <c r="E33" s="40" t="s">
         <v>262</v>
       </c>
-      <c r="F33" s="31" t="s">
+      <c r="F33" s="28" t="s">
         <v>181</v>
       </c>
-      <c r="G33" s="31"/>
-      <c r="H33" s="31" t="s">
+      <c r="G33" s="28"/>
+      <c r="H33" s="28" t="s">
         <v>182</v>
       </c>
       <c r="I33" s="6"/>
@@ -3811,22 +3775,22 @@
       </c>
     </row>
     <row r="34" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A34" s="31">
+      <c r="A34" s="28">
         <v>67</v>
       </c>
-      <c r="B34" s="31"/>
-      <c r="C34" s="31"/>
-      <c r="D34" s="31"/>
-      <c r="E34" s="48" t="s">
+      <c r="B34" s="28"/>
+      <c r="C34" s="28"/>
+      <c r="D34" s="28"/>
+      <c r="E34" s="40" t="s">
         <v>262</v>
       </c>
-      <c r="F34" s="30" t="s">
+      <c r="F34" s="27" t="s">
         <v>185</v>
       </c>
-      <c r="G34" s="31" t="s">
+      <c r="G34" s="28" t="s">
         <v>52</v>
       </c>
-      <c r="H34" s="31" t="s">
+      <c r="H34" s="28" t="s">
         <v>186</v>
       </c>
       <c r="I34" s="6"/>
@@ -3872,26 +3836,26 @@
       </c>
     </row>
     <row r="35" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A35" s="33">
+      <c r="A35" s="28">
         <v>69</v>
       </c>
-      <c r="B35" s="54" t="s">
-        <v>27</v>
-      </c>
-      <c r="C35" s="33" t="s">
-        <v>27</v>
-      </c>
-      <c r="D35" s="61"/>
-      <c r="E35" s="48" t="s">
+      <c r="B35" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="C35" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="D35" s="59"/>
+      <c r="E35" s="60" t="s">
         <v>262</v>
       </c>
-      <c r="F35" s="34" t="s">
+      <c r="F35" s="27" t="s">
         <v>189</v>
       </c>
-      <c r="G35" s="33" t="s">
+      <c r="G35" s="28" t="s">
         <v>52</v>
       </c>
-      <c r="H35" s="33" t="s">
+      <c r="H35" s="28" t="s">
         <v>190</v>
       </c>
       <c r="I35" s="6"/>
@@ -3920,11 +3884,11 @@
       <c r="R35" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="S35" s="80" t="s">
-        <v>284</v>
-      </c>
-      <c r="T35" s="75" t="s">
-        <v>272</v>
+      <c r="S35" s="52" t="s">
+        <v>282</v>
+      </c>
+      <c r="T35" s="48" t="s">
+        <v>270</v>
       </c>
       <c r="U35" s="8" t="s">
         <v>27</v>
@@ -3943,27 +3907,27 @@
       </c>
     </row>
     <row r="36" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A36" s="28">
+      <c r="A36" s="11">
         <v>70</v>
       </c>
-      <c r="B36" s="53" t="s">
-        <v>27</v>
-      </c>
-      <c r="C36" s="53"/>
-      <c r="D36" s="60" t="s">
+      <c r="B36" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C36" s="11"/>
+      <c r="D36" s="57" t="s">
         <v>27</v>
       </c>
       <c r="E36" s="9" t="s">
         <v>261</v>
       </c>
-      <c r="F36" s="28" t="s">
+      <c r="F36" s="11" t="s">
         <v>193</v>
       </c>
-      <c r="G36" s="28" t="s">
+      <c r="G36" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="H36" s="28" t="s">
-        <v>268</v>
+      <c r="H36" s="11" t="s">
+        <v>290</v>
       </c>
       <c r="I36" s="6"/>
       <c r="J36" s="7"/>
@@ -3979,7 +3943,7 @@
       <c r="N36" s="8" t="s">
         <v>194</v>
       </c>
-      <c r="O36" s="56" t="s">
+      <c r="O36" s="44" t="s">
         <v>195</v>
       </c>
       <c r="P36" s="8" t="s">
@@ -3988,8 +3952,8 @@
       <c r="Q36" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="S36" s="79" t="s">
-        <v>282</v>
+      <c r="S36" s="51" t="s">
+        <v>280</v>
       </c>
       <c r="U36" s="8" t="s">
         <v>27</v>
@@ -4008,18 +3972,18 @@
       </c>
     </row>
     <row r="37" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A37" s="26">
+      <c r="A37" s="24">
         <v>72</v>
       </c>
-      <c r="B37" s="26"/>
-      <c r="C37" s="26"/>
-      <c r="D37" s="26"/>
-      <c r="E37" s="26"/>
-      <c r="F37" s="27" t="s">
+      <c r="B37" s="24"/>
+      <c r="C37" s="24"/>
+      <c r="D37" s="24"/>
+      <c r="E37" s="24"/>
+      <c r="F37" s="25" t="s">
         <v>196</v>
       </c>
-      <c r="G37" s="26"/>
-      <c r="H37" s="26"/>
+      <c r="G37" s="24"/>
+      <c r="H37" s="24"/>
       <c r="I37" s="6"/>
       <c r="J37" s="7"/>
       <c r="K37" s="8">
@@ -4063,63 +4027,63 @@
       </c>
     </row>
     <row r="38" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A38" s="35">
+      <c r="A38" s="61">
         <v>101</v>
       </c>
-      <c r="B38" s="52" t="s">
-        <v>27</v>
-      </c>
-      <c r="C38" s="37" t="s">
-        <v>27</v>
-      </c>
-      <c r="D38" s="62"/>
-      <c r="E38" s="52" t="s">
-        <v>263</v>
-      </c>
-      <c r="F38" s="36" t="s">
+      <c r="B38" s="62" t="s">
+        <v>27</v>
+      </c>
+      <c r="C38" s="62" t="s">
+        <v>27</v>
+      </c>
+      <c r="D38" s="63"/>
+      <c r="E38" s="62" t="s">
+        <v>260</v>
+      </c>
+      <c r="F38" s="64" t="s">
         <v>243</v>
       </c>
-      <c r="G38" s="37" t="s">
+      <c r="G38" s="62" t="s">
         <v>52</v>
       </c>
-      <c r="H38" s="37" t="s">
+      <c r="H38" s="62" t="s">
         <v>199</v>
       </c>
       <c r="I38" s="6"/>
       <c r="J38" s="7"/>
-      <c r="O38" s="56" t="s">
+      <c r="O38" s="44" t="s">
         <v>244</v>
       </c>
       <c r="P38" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="S38" s="79" t="s">
-        <v>270</v>
-      </c>
-      <c r="V38" s="64">
+      <c r="S38" s="51" t="s">
+        <v>268</v>
+      </c>
+      <c r="V38" s="47">
         <v>0</v>
       </c>
-      <c r="W38" s="64">
+      <c r="W38" s="47">
         <v>124</v>
       </c>
-      <c r="X38" s="64">
+      <c r="X38" s="47">
         <v>124</v>
       </c>
-      <c r="Y38" s="64" t="s">
+      <c r="Y38" s="47" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="39" spans="1:25" ht="14.65" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A39" s="38">
+      <c r="A39" s="31">
         <v>102</v>
       </c>
-      <c r="B39" s="38"/>
-      <c r="C39" s="38"/>
-      <c r="D39" s="38"/>
-      <c r="E39" s="57" t="s">
+      <c r="B39" s="31"/>
+      <c r="C39" s="31"/>
+      <c r="D39" s="31"/>
+      <c r="E39" s="45" t="s">
         <v>263</v>
       </c>
-      <c r="F39" s="39" t="s">
+      <c r="F39" s="32" t="s">
         <v>200</v>
       </c>
       <c r="G39" s="17" t="s">
@@ -4135,121 +4099,121 @@
       </c>
     </row>
     <row r="40" spans="1:25" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A40" s="40">
+      <c r="A40" s="65">
         <v>103</v>
       </c>
-      <c r="B40" s="52" t="s">
-        <v>27</v>
-      </c>
-      <c r="C40" s="37" t="s">
-        <v>27</v>
-      </c>
-      <c r="D40" s="62"/>
-      <c r="E40" s="52" t="s">
+      <c r="B40" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="C40" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="D40" s="54"/>
+      <c r="E40" s="17" t="s">
         <v>263</v>
       </c>
-      <c r="F40" s="74" t="s">
+      <c r="F40" s="66" t="s">
         <v>247</v>
       </c>
-      <c r="G40" s="37" t="s">
+      <c r="G40" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="H40" s="37" t="s">
+      <c r="H40" s="17" t="s">
         <v>202</v>
       </c>
       <c r="I40" s="6"/>
       <c r="J40" s="7"/>
-      <c r="O40" s="56" t="s">
+      <c r="O40" s="44" t="s">
         <v>246</v>
       </c>
-      <c r="S40" s="80" t="s">
-        <v>271</v>
-      </c>
-      <c r="V40" s="64">
+      <c r="S40" s="52" t="s">
+        <v>269</v>
+      </c>
+      <c r="V40" s="47">
         <v>34</v>
       </c>
-      <c r="W40" s="64">
+      <c r="W40" s="47">
         <v>188</v>
       </c>
-      <c r="X40" s="64">
+      <c r="X40" s="47">
         <v>154</v>
       </c>
-      <c r="Y40" s="64" t="s">
+      <c r="Y40" s="47" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="41" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A41" s="37">
+      <c r="A41" s="17">
         <v>104</v>
       </c>
-      <c r="B41" s="52" t="s">
-        <v>27</v>
-      </c>
-      <c r="C41" s="37" t="s">
-        <v>27</v>
-      </c>
-      <c r="D41" s="37"/>
-      <c r="E41" s="52" t="s">
+      <c r="B41" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="C41" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="D41" s="17"/>
+      <c r="E41" s="17" t="s">
         <v>263</v>
       </c>
-      <c r="F41" s="37" t="s">
+      <c r="F41" s="17" t="s">
         <v>255</v>
       </c>
-      <c r="G41" s="37" t="s">
+      <c r="G41" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="H41" s="37" t="s">
+      <c r="H41" s="17" t="s">
         <v>202</v>
       </c>
       <c r="I41" s="6"/>
       <c r="J41" s="7"/>
-      <c r="O41" s="41" t="s">
+      <c r="O41" s="33" t="s">
         <v>203</v>
       </c>
       <c r="P41" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="S41" s="79" t="s">
-        <v>277</v>
-      </c>
-      <c r="T41" s="75" t="s">
-        <v>273</v>
-      </c>
-      <c r="V41" s="77">
+      <c r="S41" s="51" t="s">
+        <v>275</v>
+      </c>
+      <c r="T41" s="48" t="s">
+        <v>271</v>
+      </c>
+      <c r="V41" s="49">
         <v>0</v>
       </c>
-      <c r="W41" s="77">
+      <c r="W41" s="49">
         <v>171</v>
       </c>
-      <c r="X41" s="64">
+      <c r="X41" s="47">
         <v>171</v>
       </c>
-      <c r="Y41" s="64" t="s">
+      <c r="Y41" s="47" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="42" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A42" s="83">
+      <c r="A42" s="53">
         <v>105</v>
       </c>
       <c r="B42" s="17"/>
       <c r="C42" s="17"/>
-      <c r="D42" s="84"/>
+      <c r="D42" s="54"/>
       <c r="E42" s="17" t="s">
         <v>263</v>
       </c>
       <c r="F42" s="17" t="s">
         <v>251</v>
       </c>
-      <c r="G42" s="37" t="s">
+      <c r="G42" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="H42" s="37" t="s">
-        <v>269</v>
+      <c r="H42" s="30" t="s">
+        <v>267</v>
       </c>
       <c r="I42" s="6"/>
       <c r="J42" s="7"/>
-      <c r="O42" s="42" t="s">
+      <c r="O42" s="34" t="s">
         <v>204</v>
       </c>
       <c r="P42" s="8" t="s">
@@ -4260,37 +4224,37 @@
       </c>
     </row>
     <row r="43" spans="1:25" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A43" s="66">
+      <c r="A43" s="67">
         <v>106</v>
       </c>
-      <c r="B43" s="65" t="s">
-        <v>27</v>
-      </c>
-      <c r="C43" s="65" t="s">
-        <v>27</v>
-      </c>
-      <c r="D43" s="68"/>
-      <c r="E43" s="65" t="s">
+      <c r="B43" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D43" s="56"/>
+      <c r="E43" s="4" t="s">
         <v>260</v>
       </c>
-      <c r="F43" s="66" t="s">
+      <c r="F43" s="67" t="s">
         <v>248</v>
       </c>
-      <c r="G43" s="66" t="s">
+      <c r="G43" s="67" t="s">
         <v>31</v>
       </c>
-      <c r="H43" s="66" t="s">
+      <c r="H43" s="67" t="s">
         <v>205</v>
       </c>
       <c r="I43" s="6"/>
       <c r="J43" s="7"/>
-      <c r="O43" s="56" t="s">
+      <c r="O43" s="44" t="s">
         <v>206</v>
       </c>
       <c r="P43" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="S43" s="79" t="s">
+      <c r="S43" s="51" t="s">
         <v>207</v>
       </c>
       <c r="V43">
@@ -4302,12 +4266,12 @@
       <c r="X43" s="8">
         <v>160</v>
       </c>
-      <c r="Y43" s="64" t="s">
+      <c r="Y43" s="47" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="44" spans="1:25" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A44" s="83">
+      <c r="A44" s="53">
         <v>107</v>
       </c>
       <c r="B44" s="17"/>
@@ -4319,15 +4283,15 @@
       <c r="F44" s="17" t="s">
         <v>249</v>
       </c>
-      <c r="G44" s="37" t="s">
+      <c r="G44" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="H44" s="37" t="s">
+      <c r="H44" s="30" t="s">
         <v>208</v>
       </c>
       <c r="I44" s="6"/>
       <c r="J44" s="7"/>
-      <c r="O44" s="42" t="s">
+      <c r="O44" s="34" t="s">
         <v>209</v>
       </c>
       <c r="S44" s="8" t="s">
@@ -4341,7 +4305,7 @@
       <c r="B45" s="17"/>
       <c r="C45" s="17"/>
       <c r="D45" s="17"/>
-      <c r="E45" s="57" t="s">
+      <c r="E45" s="45" t="s">
         <v>263</v>
       </c>
       <c r="F45" s="17" t="s">
@@ -4353,7 +4317,7 @@
       <c r="H45" s="17"/>
       <c r="I45" s="6"/>
       <c r="J45" s="7"/>
-      <c r="O45" s="42" t="s">
+      <c r="O45" s="34" t="s">
         <v>211</v>
       </c>
       <c r="S45" s="8" t="s">
@@ -4361,13 +4325,13 @@
       </c>
     </row>
     <row r="46" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A46" s="43">
+      <c r="A46" s="35">
         <v>109</v>
       </c>
-      <c r="B46" s="43"/>
-      <c r="C46" s="43"/>
-      <c r="D46" s="43"/>
-      <c r="E46" s="57" t="s">
+      <c r="B46" s="35"/>
+      <c r="C46" s="35"/>
+      <c r="D46" s="35"/>
+      <c r="E46" s="45" t="s">
         <v>263</v>
       </c>
       <c r="F46" s="17" t="s">
@@ -4381,7 +4345,7 @@
       </c>
       <c r="I46" s="6"/>
       <c r="J46" s="7"/>
-      <c r="O46" s="42" t="s">
+      <c r="O46" s="34" t="s">
         <v>215</v>
       </c>
       <c r="S46" s="8" t="s">
@@ -4389,37 +4353,37 @@
       </c>
     </row>
     <row r="47" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A47" s="37">
+      <c r="A47" s="17">
         <v>110</v>
       </c>
-      <c r="B47" s="52" t="s">
-        <v>27</v>
-      </c>
-      <c r="C47" s="37" t="s">
-        <v>27</v>
-      </c>
-      <c r="D47" s="62"/>
-      <c r="E47" s="52" t="s">
+      <c r="B47" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="C47" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="D47" s="54"/>
+      <c r="E47" s="17" t="s">
         <v>263</v>
       </c>
-      <c r="F47" s="37" t="s">
+      <c r="F47" s="17" t="s">
         <v>256</v>
       </c>
-      <c r="G47" s="37" t="s">
+      <c r="G47" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="H47" s="37" t="s">
+      <c r="H47" s="17" t="s">
         <v>217</v>
       </c>
       <c r="I47" s="6"/>
       <c r="J47" s="7"/>
-      <c r="O47" s="56" t="s">
+      <c r="O47" s="44" t="s">
         <v>218</v>
       </c>
       <c r="P47" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="S47" s="79" t="s">
+      <c r="S47" s="51" t="s">
         <v>219</v>
       </c>
       <c r="V47">
@@ -4428,21 +4392,21 @@
       <c r="W47">
         <v>84</v>
       </c>
-      <c r="X47" s="64">
+      <c r="X47" s="47">
         <v>61</v>
       </c>
-      <c r="Y47" s="64" t="s">
+      <c r="Y47" s="47" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="48" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A48" s="43">
+      <c r="A48" s="35">
         <v>111</v>
       </c>
-      <c r="B48" s="43"/>
-      <c r="C48" s="43"/>
-      <c r="D48" s="43"/>
-      <c r="E48" s="57" t="s">
+      <c r="B48" s="35"/>
+      <c r="C48" s="35"/>
+      <c r="D48" s="35"/>
+      <c r="E48" s="45" t="s">
         <v>263</v>
       </c>
       <c r="F48" s="17" t="s">
@@ -4454,173 +4418,173 @@
       <c r="H48" s="17"/>
       <c r="I48" s="6"/>
       <c r="J48" s="7"/>
-      <c r="O48" s="42" t="s">
+      <c r="O48" s="34" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="49" spans="1:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A49" s="37">
+      <c r="A49" s="62">
         <v>112</v>
       </c>
-      <c r="B49" s="52" t="s">
-        <v>27</v>
-      </c>
-      <c r="C49" s="37" t="s">
-        <v>27</v>
-      </c>
-      <c r="D49" s="62"/>
-      <c r="E49" s="52" t="s">
+      <c r="B49" s="62" t="s">
+        <v>27</v>
+      </c>
+      <c r="C49" s="62" t="s">
+        <v>27</v>
+      </c>
+      <c r="D49" s="63"/>
+      <c r="E49" s="62" t="s">
+        <v>260</v>
+      </c>
+      <c r="F49" s="62" t="s">
+        <v>257</v>
+      </c>
+      <c r="G49" s="62" t="s">
+        <v>31</v>
+      </c>
+      <c r="H49" s="62" t="s">
+        <v>222</v>
+      </c>
+      <c r="I49" s="36"/>
+      <c r="J49" s="37"/>
+      <c r="K49" s="38"/>
+      <c r="L49" s="38"/>
+      <c r="M49" s="38"/>
+      <c r="N49" s="38"/>
+      <c r="O49" s="22" t="s">
+        <v>223</v>
+      </c>
+      <c r="P49" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q49" s="38"/>
+      <c r="R49" s="38"/>
+      <c r="S49" s="51" t="s">
+        <v>283</v>
+      </c>
+      <c r="T49" s="38"/>
+      <c r="U49" s="38"/>
+      <c r="V49" s="50">
+        <v>0</v>
+      </c>
+      <c r="W49" s="47">
+        <v>216</v>
+      </c>
+      <c r="X49" s="47">
+        <v>216</v>
+      </c>
+      <c r="Y49" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z49" s="38"/>
+      <c r="AA49" s="38"/>
+      <c r="AB49" s="38"/>
+    </row>
+    <row r="50" spans="1:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A50" s="35">
+        <v>113</v>
+      </c>
+      <c r="B50" s="46"/>
+      <c r="C50" s="46"/>
+      <c r="D50" s="46"/>
+      <c r="E50" s="45" t="s">
         <v>263</v>
       </c>
-      <c r="F49" s="37" t="s">
-        <v>257</v>
-      </c>
-      <c r="G49" s="37" t="s">
+      <c r="F50" s="39" t="s">
+        <v>264</v>
+      </c>
+      <c r="G50" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="H49" s="37" t="s">
-        <v>222</v>
-      </c>
-      <c r="I49" s="44"/>
-      <c r="J49" s="45"/>
-      <c r="K49" s="46"/>
-      <c r="L49" s="46"/>
-      <c r="M49" s="46"/>
-      <c r="N49" s="46"/>
-      <c r="O49" s="23" t="s">
-        <v>223</v>
-      </c>
-      <c r="P49" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q49" s="46"/>
-      <c r="R49" s="46"/>
-      <c r="S49" s="79" t="s">
-        <v>285</v>
-      </c>
-      <c r="T49" s="46"/>
-      <c r="U49" s="46"/>
-      <c r="V49" s="78">
-        <v>0</v>
-      </c>
-      <c r="W49" s="64">
-        <v>216</v>
-      </c>
-      <c r="X49" s="64">
-        <v>216</v>
-      </c>
-      <c r="Y49" s="64" t="s">
-        <v>27</v>
-      </c>
-      <c r="Z49" s="46"/>
-      <c r="AA49" s="46"/>
-      <c r="AB49" s="46"/>
-    </row>
-    <row r="50" spans="1:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A50" s="43">
-        <v>113</v>
-      </c>
-      <c r="B50" s="59"/>
-      <c r="C50" s="59"/>
-      <c r="D50" s="59"/>
-      <c r="E50" s="57" t="s">
-        <v>263</v>
-      </c>
-      <c r="F50" s="47" t="s">
-        <v>264</v>
-      </c>
-      <c r="G50" s="43" t="s">
-        <v>31</v>
-      </c>
-      <c r="H50" s="43" t="s">
+      <c r="H50" s="35" t="s">
         <v>224</v>
       </c>
       <c r="I50" s="6"/>
       <c r="J50" s="7"/>
-      <c r="O50" s="42" t="s">
+      <c r="O50" s="34" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="51" spans="1:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A51" s="40">
+      <c r="A51" s="65">
         <v>114</v>
       </c>
-      <c r="B51" s="40" t="s">
-        <v>27</v>
-      </c>
-      <c r="C51" s="40" t="s">
-        <v>27</v>
-      </c>
-      <c r="D51" s="81"/>
-      <c r="E51" s="37" t="s">
+      <c r="B51" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C51" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="D51" s="68"/>
+      <c r="E51" s="17" t="s">
         <v>263</v>
       </c>
-      <c r="F51" s="82" t="s">
+      <c r="F51" s="39" t="s">
         <v>265</v>
       </c>
-      <c r="G51" s="59" t="s">
+      <c r="G51" s="65" t="s">
         <v>31</v>
       </c>
-      <c r="H51" s="76" t="s">
-        <v>274</v>
+      <c r="H51" s="65" t="s">
+        <v>272</v>
       </c>
       <c r="I51" s="6"/>
       <c r="J51" s="7"/>
-      <c r="O51" s="56" t="s">
+      <c r="O51" s="44" t="s">
         <v>226</v>
       </c>
       <c r="P51" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="S51" s="85" t="s">
-        <v>288</v>
+      <c r="S51" s="55" t="s">
+        <v>286</v>
       </c>
       <c r="V51">
         <v>35</v>
       </c>
-      <c r="W51" s="64">
+      <c r="W51" s="47">
         <v>137</v>
       </c>
-      <c r="X51" s="64">
+      <c r="X51" s="47">
         <v>102</v>
       </c>
-      <c r="Y51" s="64" t="s">
+      <c r="Y51" s="47" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="52" spans="1:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A52" s="24">
+      <c r="A52" s="58">
         <v>115</v>
       </c>
-      <c r="B52" s="67" t="s">
-        <v>27</v>
-      </c>
-      <c r="C52" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="D52" s="63"/>
+      <c r="B52" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="C52" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D52" s="69"/>
       <c r="E52" s="9" t="s">
         <v>261</v>
       </c>
-      <c r="F52" s="67" t="s">
+      <c r="F52" s="21" t="s">
         <v>252</v>
       </c>
-      <c r="G52" s="24" t="s">
+      <c r="G52" s="58" t="s">
         <v>31</v>
       </c>
-      <c r="H52" s="24" t="s">
-        <v>275</v>
+      <c r="H52" s="58" t="s">
+        <v>273</v>
       </c>
       <c r="I52" s="6"/>
       <c r="J52" s="7"/>
-      <c r="O52" s="41" t="s">
+      <c r="O52" s="33" t="s">
         <v>227</v>
       </c>
       <c r="P52" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="S52" s="79" t="s">
-        <v>276</v>
+      <c r="S52" s="51" t="s">
+        <v>274</v>
       </c>
       <c r="V52">
         <v>312</v>
@@ -4628,77 +4592,77 @@
       <c r="W52">
         <v>422</v>
       </c>
-      <c r="X52" s="64">
+      <c r="X52" s="47">
         <v>110</v>
       </c>
-      <c r="Y52" s="64" t="s">
+      <c r="Y52" s="47" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="53" spans="1:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A53" s="48">
+      <c r="A53" s="40">
         <v>116</v>
       </c>
-      <c r="B53" s="48"/>
-      <c r="C53" s="48"/>
-      <c r="D53" s="48"/>
-      <c r="E53" s="48" t="s">
+      <c r="B53" s="40"/>
+      <c r="C53" s="40"/>
+      <c r="D53" s="40"/>
+      <c r="E53" s="40" t="s">
         <v>262</v>
       </c>
-      <c r="F53" s="49" t="s">
+      <c r="F53" s="41" t="s">
         <v>228</v>
       </c>
-      <c r="G53" s="48" t="s">
+      <c r="G53" s="40" t="s">
         <v>176</v>
       </c>
-      <c r="H53" s="48" t="s">
+      <c r="H53" s="40" t="s">
         <v>229</v>
       </c>
       <c r="I53" s="6"/>
       <c r="J53" s="7"/>
       <c r="N53" s="8"/>
-      <c r="O53" s="42" t="s">
+      <c r="O53" s="34" t="s">
         <v>230</v>
       </c>
-      <c r="S53" s="50" t="s">
+      <c r="S53" s="42" t="s">
         <v>231</v>
       </c>
     </row>
     <row r="54" spans="1:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A54" s="51">
+      <c r="A54" s="60">
         <v>117</v>
       </c>
-      <c r="B54" s="51" t="s">
-        <v>27</v>
-      </c>
-      <c r="C54" s="51" t="s">
-        <v>27</v>
-      </c>
-      <c r="D54" s="69"/>
-      <c r="E54" s="70" t="s">
+      <c r="B54" s="60" t="s">
+        <v>27</v>
+      </c>
+      <c r="C54" s="60" t="s">
+        <v>27</v>
+      </c>
+      <c r="D54" s="70"/>
+      <c r="E54" s="60" t="s">
         <v>262</v>
       </c>
-      <c r="F54" s="51" t="s">
+      <c r="F54" s="60" t="s">
         <v>258</v>
       </c>
-      <c r="G54" s="51" t="s">
+      <c r="G54" s="60" t="s">
         <v>31</v>
       </c>
-      <c r="H54" s="51" t="s">
+      <c r="H54" s="60" t="s">
         <v>232</v>
       </c>
       <c r="I54" s="6">
         <v>0</v>
       </c>
       <c r="J54" s="7"/>
-      <c r="O54" s="56" t="s">
+      <c r="O54" s="44" t="s">
         <v>233</v>
       </c>
       <c r="P54" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="S54" s="79" t="s">
-        <v>279</v>
+      <c r="S54" s="51" t="s">
+        <v>277</v>
       </c>
       <c r="V54">
         <v>5</v>
@@ -4706,71 +4670,71 @@
       <c r="W54">
         <v>135</v>
       </c>
-      <c r="X54" s="64">
+      <c r="X54" s="47">
         <v>130</v>
       </c>
-      <c r="Y54" s="64" t="s">
+      <c r="Y54" s="47" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="55" spans="1:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A55" s="48">
+      <c r="A55" s="40">
         <v>118</v>
       </c>
-      <c r="B55" s="48"/>
-      <c r="C55" s="48"/>
-      <c r="D55" s="48"/>
-      <c r="E55" s="48" t="s">
+      <c r="B55" s="40"/>
+      <c r="C55" s="40"/>
+      <c r="D55" s="40"/>
+      <c r="E55" s="40" t="s">
         <v>262</v>
       </c>
-      <c r="F55" s="49" t="s">
+      <c r="F55" s="41" t="s">
         <v>234</v>
       </c>
-      <c r="G55" s="48" t="s">
+      <c r="G55" s="40" t="s">
         <v>176</v>
       </c>
-      <c r="H55" s="48" t="s">
+      <c r="H55" s="40" t="s">
         <v>235</v>
       </c>
       <c r="I55" s="6"/>
       <c r="J55" s="7"/>
-      <c r="O55" s="42" t="s">
+      <c r="O55" s="34" t="s">
         <v>236</v>
       </c>
     </row>
     <row r="56" spans="1:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A56" s="51">
+      <c r="A56" s="60">
         <v>119</v>
       </c>
-      <c r="B56" s="51" t="s">
-        <v>27</v>
-      </c>
-      <c r="C56" s="51" t="s">
-        <v>27</v>
-      </c>
-      <c r="D56" s="69"/>
-      <c r="E56" s="70" t="s">
+      <c r="B56" s="60" t="s">
+        <v>27</v>
+      </c>
+      <c r="C56" s="60" t="s">
+        <v>27</v>
+      </c>
+      <c r="D56" s="70"/>
+      <c r="E56" s="60" t="s">
         <v>262</v>
       </c>
-      <c r="F56" s="72" t="s">
+      <c r="F56" s="41" t="s">
         <v>253</v>
       </c>
-      <c r="G56" s="51" t="s">
+      <c r="G56" s="60" t="s">
         <v>31</v>
       </c>
-      <c r="H56" s="51" t="s">
+      <c r="H56" s="60" t="s">
         <v>237</v>
       </c>
       <c r="I56" s="6"/>
       <c r="J56" s="7"/>
-      <c r="O56" s="42" t="s">
+      <c r="O56" s="34" t="s">
         <v>238</v>
       </c>
       <c r="P56" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="S56" s="79" t="s">
-        <v>278</v>
+      <c r="S56" s="51" t="s">
+        <v>276</v>
       </c>
       <c r="V56">
         <v>10</v>
@@ -4778,46 +4742,46 @@
       <c r="W56">
         <v>160</v>
       </c>
-      <c r="X56" s="64">
+      <c r="X56" s="47">
         <v>150</v>
       </c>
-      <c r="Y56" s="64" t="s">
+      <c r="Y56" s="47" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="57" spans="1:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A57" s="51">
+      <c r="A57" s="60">
         <v>120</v>
       </c>
-      <c r="B57" s="51" t="s">
-        <v>27</v>
-      </c>
-      <c r="C57" s="51" t="s">
-        <v>27</v>
-      </c>
-      <c r="D57" s="69"/>
-      <c r="E57" s="70" t="s">
+      <c r="B57" s="60" t="s">
+        <v>27</v>
+      </c>
+      <c r="C57" s="60" t="s">
+        <v>27</v>
+      </c>
+      <c r="D57" s="70"/>
+      <c r="E57" s="60" t="s">
         <v>262</v>
       </c>
-      <c r="F57" s="72" t="s">
+      <c r="F57" s="41" t="s">
         <v>254</v>
       </c>
-      <c r="G57" s="51" t="s">
+      <c r="G57" s="60" t="s">
         <v>31</v>
       </c>
-      <c r="H57" s="51" t="s">
+      <c r="H57" s="60" t="s">
         <v>239</v>
       </c>
       <c r="I57" s="6"/>
       <c r="J57" s="7"/>
-      <c r="O57" s="56" t="s">
+      <c r="O57" s="44" t="s">
         <v>240</v>
       </c>
       <c r="P57" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="S57" s="80" t="s">
-        <v>287</v>
+      <c r="S57" s="52" t="s">
+        <v>285</v>
       </c>
       <c r="V57">
         <v>4</v>
@@ -4825,10 +4789,10 @@
       <c r="W57">
         <v>90</v>
       </c>
-      <c r="X57" s="64">
+      <c r="X57" s="47">
         <v>86</v>
       </c>
-      <c r="Y57" s="64" t="s">
+      <c r="Y57" s="47" t="s">
         <v>27</v>
       </c>
     </row>
@@ -9586,21 +9550,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100FD76100231DEBB49ACA4C116F1478A15" ma:contentTypeVersion="4" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="9a3d2e71c0e98aa2d819d404d3684a97">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="871ff5df-2620-46ed-9b99-7f24ebb6857b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c0f0fcb00e0820a9119da58c691a79d6" ns3:_="">
     <xsd:import namespace="871ff5df-2620-46ed-9b99-7f24ebb6857b"/>
@@ -9744,10 +9693,35 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E6991839-7F0F-4975-94BB-957F2545D6AA}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AB96B9AD-1DF0-4BB1-8D5F-BA0E1DAB007B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="871ff5df-2620-46ed-9b99-7f24ebb6857b"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -9769,19 +9743,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AB96B9AD-1DF0-4BB1-8D5F-BA0E1DAB007B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E6991839-7F0F-4975-94BB-957F2545D6AA}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="871ff5df-2620-46ed-9b99-7f24ebb6857b"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>